<commit_message>
put the results for bayesian analysis for use case weights in the data/temp folder. In the future statistic analysis results should be put here
</commit_message>
<xml_diff>
--- a/data/UseCaseWeighting/UCP_DatasetV1.2.xlsx
+++ b/data/UseCaseWeighting/UCP_DatasetV1.2.xlsx
@@ -13,13 +13,14 @@
   </bookViews>
   <sheets>
     <sheet name="UCP_DatasetV1.2" sheetId="1" r:id="rId1"/>
+    <sheet name="UCC Data Points" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t>Project_No</t>
   </si>
@@ -145,6 +146,42 @@
   </si>
   <si>
     <t>s17_tikiman_go</t>
+  </si>
+  <si>
+    <t>Proj.</t>
+  </si>
+  <si>
+    <t>Effort</t>
+  </si>
+  <si>
+    <t>EF</t>
+  </si>
+  <si>
+    <t>UC_1</t>
+  </si>
+  <si>
+    <t>UC_2</t>
+  </si>
+  <si>
+    <t>UC_3</t>
+  </si>
+  <si>
+    <t>UC_4</t>
+  </si>
+  <si>
+    <t>UC_5</t>
+  </si>
+  <si>
+    <t>UC_6</t>
+  </si>
+  <si>
+    <t>UC_7</t>
+  </si>
+  <si>
+    <t>UC_8</t>
+  </si>
+  <si>
+    <t>UC_9</t>
   </si>
 </sst>
 </file>
@@ -958,15 +995,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -1104,11 +1144,11 @@
         <v>3</v>
       </c>
       <c r="J3" s="1">
-        <f t="shared" ref="J3:J26" si="0">G3*5+H3*10+I3*15</f>
+        <f t="shared" ref="J3:J35" si="0">G3*5+H3*10+I3*15</f>
         <v>115</v>
       </c>
       <c r="K3" s="1">
-        <f t="shared" ref="K3:K26" si="1">J3+F3</f>
+        <f t="shared" ref="K3:K27" si="1">J3+F3</f>
         <v>126</v>
       </c>
       <c r="L3" s="1">
@@ -1118,7 +1158,7 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="N3" s="1">
-        <f t="shared" ref="N3:N26" si="2">K3*L3*M3</f>
+        <f t="shared" ref="N3:N35" si="2">K3*L3*M3</f>
         <v>116.235</v>
       </c>
       <c r="O3" s="1">
@@ -2327,7 +2367,7 @@
         <v>140</v>
       </c>
       <c r="K26" s="1">
-        <f t="shared" si="1"/>
+        <f>J26+F26</f>
         <v>143</v>
       </c>
       <c r="L26" s="1">
@@ -2345,6 +2385,714 @@
       </c>
       <c r="P26" s="1">
         <v>23.940230629999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <f>1*C27+2*D27+3*E27</f>
+        <v>3</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>2</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27" s="1">
+        <f>G27*5+H27*10+I27*15</f>
+        <v>35</v>
+      </c>
+      <c r="K27" s="1">
+        <f t="shared" ref="K27:K35" si="3">J27+F27</f>
+        <v>38</v>
+      </c>
+      <c r="L27">
+        <v>1.03</v>
+      </c>
+      <c r="M27">
+        <v>2.25</v>
+      </c>
+      <c r="N27" s="1">
+        <f t="shared" si="2"/>
+        <v>88.064999999999998</v>
+      </c>
+      <c r="O27">
+        <v>2981.4933332999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <f t="shared" ref="F28:F35" si="4">1*C28+2*D28+3*E28</f>
+        <v>3</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28" s="1">
+        <f>G28*5+H28*10+I28*15</f>
+        <v>20</v>
+      </c>
+      <c r="K28" s="1">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="L28">
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="M28">
+        <v>2.4499999999999997</v>
+      </c>
+      <c r="N28" s="1">
+        <f t="shared" si="2"/>
+        <v>56.63174999999999</v>
+      </c>
+      <c r="O28">
+        <v>58.730999999999995</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>18</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29" s="1">
+        <f>G29*5+H29*10+I29*15</f>
+        <v>90</v>
+      </c>
+      <c r="K29" s="1">
+        <f t="shared" si="3"/>
+        <v>91</v>
+      </c>
+      <c r="L29">
+        <v>1.0160000000000002</v>
+      </c>
+      <c r="M29">
+        <v>2.25</v>
+      </c>
+      <c r="N29" s="1">
+        <f t="shared" si="2"/>
+        <v>208.02600000000004</v>
+      </c>
+      <c r="O29">
+        <v>285.51375000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="K30" s="1">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="L30">
+        <v>1.0199999999999998</v>
+      </c>
+      <c r="M30">
+        <v>2.0833333333333335</v>
+      </c>
+      <c r="N30" s="1">
+        <f t="shared" si="2"/>
+        <v>72.249999999999986</v>
+      </c>
+      <c r="O30">
+        <v>104.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>3</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31" s="1">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="K31" s="1">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="L31">
+        <v>1.0287500000000001</v>
+      </c>
+      <c r="M31">
+        <v>2.25</v>
+      </c>
+      <c r="N31" s="1">
+        <f t="shared" si="2"/>
+        <v>108.7903125</v>
+      </c>
+      <c r="O31">
+        <v>124.90875</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>6</v>
+      </c>
+      <c r="B32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="G32">
+        <v>2</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="K32" s="1">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="L32">
+        <v>1.02125</v>
+      </c>
+      <c r="M32">
+        <v>2.4</v>
+      </c>
+      <c r="N32" s="1">
+        <f t="shared" si="2"/>
+        <v>63.725999999999992</v>
+      </c>
+      <c r="O32">
+        <v>115.46024999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>7</v>
+      </c>
+      <c r="B33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33">
+        <v>8</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>5</v>
+      </c>
+      <c r="I33">
+        <v>2</v>
+      </c>
+      <c r="J33" s="1">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="K33" s="1">
+        <f t="shared" si="3"/>
+        <v>93</v>
+      </c>
+      <c r="L33">
+        <v>1.0306250000000001</v>
+      </c>
+      <c r="M33">
+        <v>2.25</v>
+      </c>
+      <c r="N33" s="1">
+        <f t="shared" si="2"/>
+        <v>215.65828125000002</v>
+      </c>
+      <c r="O33">
+        <v>9678.3333332999991</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>8</v>
+      </c>
+      <c r="B34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="G34">
+        <v>22</v>
+      </c>
+      <c r="H34">
+        <v>2</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34" s="1">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="K34" s="1">
+        <f t="shared" si="3"/>
+        <v>132</v>
+      </c>
+      <c r="L34">
+        <v>1.0156250000000002</v>
+      </c>
+      <c r="M34">
+        <v>2.25</v>
+      </c>
+      <c r="N34" s="1">
+        <f t="shared" si="2"/>
+        <v>301.64062500000006</v>
+      </c>
+      <c r="O34">
+        <v>9559.8866667000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>9</v>
+      </c>
+      <c r="B35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="G35">
+        <v>3</v>
+      </c>
+      <c r="H35">
+        <v>2</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35" s="1">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="K35" s="1">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="L35">
+        <v>1.0129999999999999</v>
+      </c>
+      <c r="M35">
+        <v>2.3899999999999997</v>
+      </c>
+      <c r="N35" s="1">
+        <f t="shared" si="2"/>
+        <v>104.10600999999998</v>
+      </c>
+      <c r="O35">
+        <v>174.74625</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1.03</v>
+      </c>
+      <c r="F2">
+        <v>2.25</v>
+      </c>
+      <c r="G2">
+        <v>2981.4933332999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="F3">
+        <v>2.4499999999999997</v>
+      </c>
+      <c r="G3">
+        <v>58.730999999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1.0160000000000002</v>
+      </c>
+      <c r="F4">
+        <v>2.25</v>
+      </c>
+      <c r="G4">
+        <v>285.51375000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1.0199999999999998</v>
+      </c>
+      <c r="F5">
+        <v>2.0833333333333335</v>
+      </c>
+      <c r="G5">
+        <v>104.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1.0287500000000001</v>
+      </c>
+      <c r="F6">
+        <v>2.25</v>
+      </c>
+      <c r="G6">
+        <v>124.90875</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1.02125</v>
+      </c>
+      <c r="F7">
+        <v>2.4</v>
+      </c>
+      <c r="G7">
+        <v>115.46024999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>1.0306250000000001</v>
+      </c>
+      <c r="F8">
+        <v>2.25</v>
+      </c>
+      <c r="G8">
+        <v>9678.3333332999991</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>22</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1.0156250000000002</v>
+      </c>
+      <c r="F9">
+        <v>2.25</v>
+      </c>
+      <c r="G9">
+        <v>9559.8866667000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1.0129999999999999</v>
+      </c>
+      <c r="F10">
+        <v>2.3899999999999997</v>
+      </c>
+      <c r="G10">
+        <v>174.74625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>